<commit_message>
fix: masuk reten gender baru yg dah centerkan beberapa font
</commit_message>
<xml_diff>
--- a/public/exports/GENDER.xlsx
+++ b/public/exports/GENDER.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calypso\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calypso\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B3AD2B-3120-4D6C-9C24-B33206FEA1FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA237F7B-AECA-4783-B5FA-8295B98CB1E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FAC87BEB-405F-40ED-9A81-8A6D5ED91B05}"/>
   </bookViews>
@@ -343,7 +343,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -413,9 +413,6 @@
     <xf numFmtId="1" fontId="5" fillId="6" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -774,7 +771,7 @@
   <dimension ref="A1:Y14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="Y7" sqref="X7:Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,41 +846,41 @@
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28" t="s">
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="35" t="s">
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="36"/>
-      <c r="Q7" s="37"/>
-      <c r="R7" s="31" t="s">
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="36"/>
+      <c r="R7" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="S7" s="32"/>
-      <c r="T7" s="32"/>
-      <c r="U7" s="32"/>
-      <c r="V7" s="33"/>
-      <c r="W7" s="34" t="s">
+      <c r="S7" s="31"/>
+      <c r="T7" s="31"/>
+      <c r="U7" s="31"/>
+      <c r="V7" s="32"/>
+      <c r="W7" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="X7" s="24" t="s">
+      <c r="X7" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="Y7" s="24" t="s">
+      <c r="Y7" s="33" t="s">
         <v>9</v>
       </c>
     </row>
@@ -950,9 +947,9 @@
       <c r="V8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="W8" s="34"/>
-      <c r="X8" s="24"/>
-      <c r="Y8" s="24"/>
+      <c r="W8" s="33"/>
+      <c r="X8" s="33"/>
+      <c r="Y8" s="33"/>
     </row>
     <row r="9" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">

</xml_diff>